<commit_message>
ejercicios con objetos elements
</commit_message>
<xml_diff>
--- a/documentacion-proyecto-final/grupos-codigo-8-final.xlsx
+++ b/documentacion-proyecto-final/grupos-codigo-8-final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodiGo\codigo-virtual-8\documentacion-proyecto-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCB3B11-93AF-4D1E-A2F7-F3EDD8A1332D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A35DCBE-E4CA-4265-8DA7-F343E93BCEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F133B3A8-4619-44B0-8334-4AE25496A338}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{F133B3A8-4619-44B0-8334-4AE25496A338}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="127">
   <si>
     <t>Nombre</t>
   </si>
@@ -397,6 +397,18 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>NETWORK</t>
+  </si>
+  <si>
+    <t>Ecommerce productos domesticos</t>
+  </si>
+  <si>
+    <t>Web profesional influencer</t>
+  </si>
+  <si>
+    <t>Software financiero</t>
   </si>
 </sst>
 </file>
@@ -449,7 +461,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -519,6 +531,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -607,7 +625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -763,9 +781,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -814,6 +829,25 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1129,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB20FB3-F63C-48E3-B60B-37F356E4ADA7}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,7 +1178,7 @@
     <col min="6" max="6" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1167,7 +1201,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>24</v>
       </c>
@@ -1190,7 +1224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1213,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>15</v>
       </c>
@@ -1236,7 +1270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10</v>
       </c>
@@ -1258,8 +1292,11 @@
       <c r="G5" s="38">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="76" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>23</v>
       </c>
@@ -1275,14 +1312,15 @@
       <c r="E6" s="41">
         <v>931060610</v>
       </c>
-      <c r="F6" s="75" t="s">
+      <c r="F6" s="74" t="s">
         <v>94</v>
       </c>
       <c r="G6" s="38">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="76"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1304,8 +1342,9 @@
       <c r="G7" s="38">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="76"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>13</v>
       </c>
@@ -1327,8 +1366,9 @@
       <c r="G8" s="38">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="76"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>14</v>
       </c>
@@ -1351,7 +1391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>20</v>
       </c>
@@ -1374,7 +1414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>22</v>
       </c>
@@ -1397,7 +1437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1420,7 +1460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1442,8 +1482,11 @@
       <c r="G13" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="76" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>25</v>
       </c>
@@ -1465,8 +1508,9 @@
       <c r="G14" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="76"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1488,8 +1532,9 @@
       <c r="G15" s="54">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="76"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>17</v>
       </c>
@@ -1511,31 +1556,32 @@
       <c r="G16" s="54">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="76"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>18</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D17" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="57">
+      <c r="E17" s="79">
         <v>975000583</v>
       </c>
-      <c r="F17" s="53" t="s">
+      <c r="F17" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="54">
+      <c r="G17" s="81">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>21</v>
       </c>
@@ -1557,8 +1603,11 @@
       <c r="G18" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="76" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>29</v>
       </c>
@@ -1571,7 +1620,7 @@
       <c r="D19" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="58">
+      <c r="E19" s="57">
         <v>984682719</v>
       </c>
       <c r="F19" s="17" t="s">
@@ -1580,8 +1629,9 @@
       <c r="G19" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="76"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>12</v>
       </c>
@@ -1603,8 +1653,9 @@
       <c r="G20" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="76"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>16</v>
       </c>
@@ -1617,7 +1668,7 @@
       <c r="D21" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="59">
+      <c r="E21" s="58">
         <v>959518744</v>
       </c>
       <c r="F21" s="11" t="s">
@@ -1626,8 +1677,9 @@
       <c r="G21" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="76"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>27</v>
       </c>
@@ -1649,8 +1701,11 @@
       <c r="G22" s="22">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="75" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>28</v>
       </c>
@@ -1672,8 +1727,9 @@
       <c r="G23" s="22">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H23" s="75"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1695,8 +1751,9 @@
       <c r="G24" s="22">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="75"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1719,7 +1776,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1742,7 +1799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1765,72 +1822,72 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="61" t="s">
+      <c r="C28" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="61" t="s">
+      <c r="D28" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="62">
+      <c r="E28" s="61">
         <v>962395395</v>
       </c>
-      <c r="F28" s="63" t="s">
+      <c r="F28" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="64" t="s">
+      <c r="G28" s="63" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>26</v>
       </c>
-      <c r="B29" s="65" t="s">
+      <c r="B29" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="65" t="s">
         <v>103</v>
       </c>
-      <c r="D29" s="66" t="s">
+      <c r="D29" s="65" t="s">
         <v>104</v>
       </c>
-      <c r="E29" s="67">
+      <c r="E29" s="66">
         <v>926437419</v>
       </c>
-      <c r="F29" s="68" t="s">
+      <c r="F29" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="G29" s="69" t="s">
+      <c r="G29" s="68" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>19</v>
       </c>
-      <c r="B30" s="70" t="s">
+      <c r="B30" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="71" t="s">
+      <c r="C30" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="71" t="s">
+      <c r="D30" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="72">
+      <c r="E30" s="71">
         <v>941489609</v>
       </c>
-      <c r="F30" s="73" t="s">
+      <c r="F30" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="G30" s="74" t="s">
+      <c r="G30" s="73" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1840,6 +1897,12 @@
       <sortCondition ref="G1"/>
     </sortState>
   </autoFilter>
+  <mergeCells count="4">
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="H5:H8"/>
+    <mergeCell ref="H13:H16"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{FD288DA9-4712-4A29-B188-71D2D9D27CF1}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
diseño inicial barra de búsqueda climas-app
</commit_message>
<xml_diff>
--- a/documentacion-proyecto-final/grupos-codigo-8-final.xlsx
+++ b/documentacion-proyecto-final/grupos-codigo-8-final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\CodiGo\codigo-virtual-8\documentacion-proyecto-final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodiGo\codigo-virtual-8\documentacion-proyecto-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9324D2B-208F-4830-B807-28F230F587A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49388DB9-357C-44D2-9395-809C44DF6F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F133B3A8-4619-44B0-8334-4AE25496A338}"/>
+    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{F133B3A8-4619-44B0-8334-4AE25496A338}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="132">
   <si>
     <t>Nombre</t>
   </si>
@@ -418,13 +418,19 @@
   </si>
   <si>
     <t>Web tatoos</t>
+  </si>
+  <si>
+    <t>1ra Entrega</t>
+  </si>
+  <si>
+    <t>2da Entrega</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -852,13 +858,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1175,13 +1181,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB20FB3-F63C-48E3-B60B-37F356E4ADA7}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H30"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" customWidth="1"/>
@@ -1190,7 +1196,7 @@
     <col min="6" max="6" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" thickBot="1">
+    <row r="1" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1212,8 +1218,14 @@
       <c r="G1" s="3" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>24</v>
       </c>
@@ -1236,7 +1248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1259,7 +1271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>15</v>
       </c>
@@ -1282,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10</v>
       </c>
@@ -1304,11 +1316,11 @@
       <c r="G5" s="38">
         <v>2</v>
       </c>
-      <c r="H5" s="81" t="s">
+      <c r="H5" s="82" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>23</v>
       </c>
@@ -1330,9 +1342,9 @@
       <c r="G6" s="38">
         <v>2</v>
       </c>
-      <c r="H6" s="81"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H6" s="82"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1354,9 +1366,9 @@
       <c r="G7" s="38">
         <v>2</v>
       </c>
-      <c r="H7" s="81"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H7" s="82"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>13</v>
       </c>
@@ -1378,9 +1390,9 @@
       <c r="G8" s="38">
         <v>2</v>
       </c>
-      <c r="H8" s="81"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H8" s="82"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>14</v>
       </c>
@@ -1403,7 +1415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1">
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>20</v>
       </c>
@@ -1426,7 +1438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>22</v>
       </c>
@@ -1449,7 +1461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1472,7 +1484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1">
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1494,11 +1506,11 @@
       <c r="G13" s="12">
         <v>4</v>
       </c>
-      <c r="H13" s="81" t="s">
+      <c r="H13" s="82" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>25</v>
       </c>
@@ -1520,9 +1532,9 @@
       <c r="G14" s="12">
         <v>4</v>
       </c>
-      <c r="H14" s="81"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H14" s="82"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1544,9 +1556,9 @@
       <c r="G15" s="54">
         <v>4</v>
       </c>
-      <c r="H15" s="81"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H15" s="82"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>17</v>
       </c>
@@ -1568,9 +1580,9 @@
       <c r="G16" s="54">
         <v>4</v>
       </c>
-      <c r="H16" s="81"/>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H16" s="82"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>18</v>
       </c>
@@ -1593,7 +1605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>21</v>
       </c>
@@ -1615,11 +1627,11 @@
       <c r="G18" s="12">
         <v>5</v>
       </c>
-      <c r="H18" s="81" t="s">
+      <c r="H18" s="82" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>29</v>
       </c>
@@ -1641,9 +1653,9 @@
       <c r="G19" s="12">
         <v>5</v>
       </c>
-      <c r="H19" s="81"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H19" s="82"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>12</v>
       </c>
@@ -1665,9 +1677,9 @@
       <c r="G20" s="12">
         <v>5</v>
       </c>
-      <c r="H20" s="81"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H20" s="82"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>16</v>
       </c>
@@ -1689,9 +1701,9 @@
       <c r="G21" s="12">
         <v>5</v>
       </c>
-      <c r="H21" s="81"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H21" s="82"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>27</v>
       </c>
@@ -1713,11 +1725,11 @@
       <c r="G22" s="22">
         <v>10</v>
       </c>
-      <c r="H22" s="80" t="s">
+      <c r="H22" s="81" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1">
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>28</v>
       </c>
@@ -1739,9 +1751,9 @@
       <c r="G23" s="22">
         <v>10</v>
       </c>
-      <c r="H23" s="80"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H23" s="81"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1763,9 +1775,9 @@
       <c r="G24" s="22">
         <v>10</v>
       </c>
-      <c r="H24" s="80"/>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H24" s="81"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1788,7 +1800,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1">
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1811,7 +1823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1837,7 +1849,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="60.75" thickBot="1">
+    <row r="28" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1859,11 +1871,11 @@
       <c r="G28" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="H28" s="82" t="s">
+      <c r="H28" s="80" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1886,7 +1898,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30.75" thickBot="1">
+    <row r="30" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>19</v>
       </c>
@@ -1908,13 +1920,13 @@
       <c r="G30" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="H30" s="82" t="s">
+      <c r="H30" s="80" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{BC9A7E25-3A0E-4FB5-BB42-E46D30A2FAA9}">
-    <sortState ref="A2:G30">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G30">
       <sortCondition ref="G1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
subiendo proyectos en webpack
</commit_message>
<xml_diff>
--- a/documentacion-proyecto-final/grupos-codigo-8-final.xlsx
+++ b/documentacion-proyecto-final/grupos-codigo-8-final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodiGo\codigo-virtual-8\documentacion-proyecto-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49388DB9-357C-44D2-9395-809C44DF6F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB12C63-402C-4ACC-A53E-6262D5B58C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{F133B3A8-4619-44B0-8334-4AE25496A338}"/>
+    <workbookView xWindow="-57720" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{F133B3A8-4619-44B0-8334-4AE25496A338}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="133">
   <si>
     <t>Nombre</t>
   </si>
@@ -424,6 +424,9 @@
   </si>
   <si>
     <t>2da Entrega</t>
+  </si>
+  <si>
+    <t>Revisado</t>
   </si>
 </sst>
 </file>
@@ -1184,7 +1187,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,7 +1585,7 @@
       </c>
       <c r="H16" s="82"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>18</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>21</v>
       </c>
@@ -1630,8 +1633,11 @@
       <c r="H18" s="82" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I18" s="81" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>29</v>
       </c>
@@ -1654,8 +1660,9 @@
         <v>5</v>
       </c>
       <c r="H19" s="82"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="81"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>12</v>
       </c>
@@ -1678,8 +1685,9 @@
         <v>5</v>
       </c>
       <c r="H20" s="82"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I20" s="81"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>16</v>
       </c>
@@ -1702,8 +1710,9 @@
         <v>5</v>
       </c>
       <c r="H21" s="82"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I21" s="81"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>27</v>
       </c>
@@ -1728,8 +1737,11 @@
       <c r="H22" s="81" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I22" s="81" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>28</v>
       </c>
@@ -1752,8 +1764,9 @@
         <v>10</v>
       </c>
       <c r="H23" s="81"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I23" s="81"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1776,8 +1789,9 @@
         <v>10</v>
       </c>
       <c r="H24" s="81"/>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I24" s="81"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1800,7 +1814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1823,7 +1837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1849,7 +1863,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1874,8 +1888,11 @@
       <c r="H28" s="80" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1898,7 +1915,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>19</v>
       </c>
@@ -1922,6 +1939,9 @@
       </c>
       <c r="H30" s="80" t="s">
         <v>127</v>
+      </c>
+      <c r="I30" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1930,11 +1950,13 @@
       <sortCondition ref="G1"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="H22:H24"/>
     <mergeCell ref="H18:H21"/>
     <mergeCell ref="H5:H8"/>
     <mergeCell ref="H13:H16"/>
+    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="I18:I21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{FD288DA9-4712-4A29-B188-71D2D9D27CF1}"/>

</xml_diff>